<commit_message>
significant changes to nano firmware
</commit_message>
<xml_diff>
--- a/bom/swarm_b2_bom.xlsx
+++ b/bom/swarm_b2_bom.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepositories\Swarm-B2\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFDE04F-0B6B-4493-A710-ABFF1102BA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74AA81D-F14A-4353-92DC-53731EC37646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -564,24 +575,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="93.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="93.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -627,7 +638,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -635,7 +646,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -643,7 +654,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -651,7 +662,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -659,7 +670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -681,8 +692,11 @@
       <c r="G7" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -704,8 +718,15 @@
       <c r="G8" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>105</v>
+      </c>
+      <c r="I8">
+        <f>SUM(H8/4)</f>
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -728,7 +749,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -751,7 +772,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -774,7 +795,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -782,7 +803,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -805,7 +826,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -827,8 +848,11 @@
       <c r="G14" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>

</xml_diff>